<commit_message>
modificado 1 cosa del excel
</commit_message>
<xml_diff>
--- a/Finanzas/Clculo de sueldo y IESS.xlsx
+++ b/Finanzas/Clculo de sueldo y IESS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clear Minds\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clear Minds\Desktop\GitKelvin\Modulo5\Finanzas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{712C56CF-93FA-4455-8D71-8689DA3A9876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4897E7-725F-4D03-97FF-D5A52E0C9848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{32B092AB-0DF3-46EA-BFED-9C45FE22B0E0}"/>
   </bookViews>
@@ -20,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Aporte IESS Empleado</t>
   </si>
@@ -62,6 +52,9 @@
   </si>
   <si>
     <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
 </sst>
 </file>
@@ -77,15 +70,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,13 +92,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7FF83D-9F0E-4D89-983A-C8F2D2001EF4}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,195 +444,273 @@
     <col min="5" max="5" width="24" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>9.4500000000000001E-2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>0.1115</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>460</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>460</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <f>A3*$B$2</f>
         <v>43.47</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <f>A3*$C$2</f>
         <v>51.29</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <f>A3/12</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <f>$E$2/12</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <f>A3/2/12</f>
         <v>19.166666666666668</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <f>A3-B3</f>
         <v>416.53</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4">
         <f>A3+C3+D3+E3+F3</f>
         <v>607.12333333333333</v>
       </c>
+      <c r="I3" s="4">
+        <f>$H3/160</f>
+        <v>3.7945208333333333</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>500</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <f>A4*$B$2</f>
         <v>47.25</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <f>A4*$C$2</f>
         <v>55.75</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <f>A4/12</f>
         <v>41.666666666666664</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <f>$E$2/12</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <f>A4/2/12</f>
         <v>20.833333333333332</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <f>A4-B4</f>
         <v>452.75</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <f>A4+C4+D4+E4+F4</f>
         <v>656.58333333333337</v>
       </c>
+      <c r="I4" s="4">
+        <f t="shared" ref="I4:I8" si="0">$H4/160</f>
+        <v>4.1036458333333332</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>480</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <f>A5*$B$2</f>
         <v>45.36</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <f>A5*$C$2</f>
         <v>53.52</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <f>A5/12</f>
         <v>40</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <f>$E$2/12</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <f>A5/2/12</f>
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <f>A5-B5</f>
         <v>434.64</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4">
         <f>A5+C5+D5+E5+F5</f>
         <v>631.85333333333335</v>
       </c>
+      <c r="I5" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9490833333333333</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
         <v>470</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <f>A6*$B$2</f>
         <v>44.414999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <f>A6*$C$2</f>
         <v>52.405000000000001</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <f>A6/12</f>
         <v>39.166666666666664</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <f>$E$2/12</f>
         <v>38.333333333333336</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <f>A6/2/12</f>
         <v>19.583333333333332</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <f>A6-B6</f>
         <v>425.58499999999998</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <f>A6+C6+D6+E6+F6</f>
         <v>619.48833333333334</v>
       </c>
+      <c r="I6" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8718020833333333</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>4482.1400000000003</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <f>A7*$B$2</f>
         <v>423.56223000000006</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="4">
+        <f>A7*$C$2</f>
+        <v>499.75861000000003</v>
+      </c>
+      <c r="D7" s="4">
         <f>A7/12</f>
         <v>373.51166666666671</v>
       </c>
-      <c r="G7">
+      <c r="E7" s="4">
+        <f t="shared" ref="E7:E8" si="1">$E$2/12</f>
+        <v>38.333333333333336</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" ref="F7:F8" si="2">A7/2/12</f>
+        <v>186.75583333333336</v>
+      </c>
+      <c r="G7" s="4">
         <f>A7-B7</f>
         <v>4058.5777700000003</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" ref="H7:H8" si="3">A7+C7+D7+E7+F7</f>
+        <v>5580.4994433333331</v>
+      </c>
+      <c r="I7" s="4">
+        <f t="shared" si="0"/>
+        <v>34.878121520833332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>650</v>
+      </c>
+      <c r="B8" s="4">
+        <f>A8*$B$2</f>
+        <v>61.424999999999997</v>
+      </c>
+      <c r="C8" s="4">
+        <f>A8*$C$2</f>
+        <v>72.474999999999994</v>
+      </c>
+      <c r="D8" s="4">
+        <f>A8/12</f>
+        <v>54.166666666666664</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="1"/>
+        <v>38.333333333333336</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="2"/>
+        <v>27.083333333333332</v>
+      </c>
+      <c r="G8" s="4">
+        <f>A8-B8</f>
+        <v>588.57500000000005</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="3"/>
+        <v>842.05833333333339</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="0"/>
+        <v>5.2628645833333341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>